<commit_message>
Atualizado planilha para gerar histórico de pedidos e pedidos_mock.js
</commit_message>
<xml_diff>
--- a/codigo/assets/script/pedidos_mock.xlsx
+++ b/codigo/assets/script/pedidos_mock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Sprint-04\icei-pucminas-psg-si-n-tiaw-2024-1-grupo-1-reserva-de-lanches\codigo\assets\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E349590-1E5A-4071-BF05-541DFC044B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0576F13-28E1-45A3-A5BE-80B77D40EFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{4D1AFED7-1EDD-46E3-A830-15DC2F3F764B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4D1AFED7-1EDD-46E3-A830-15DC2F3F764B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>pendente</t>
-  </si>
-  <si>
-    <t>cancelado</t>
   </si>
   <si>
     <t>aprovado</t>
@@ -393,7 +390,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -404,21 +416,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -759,7 +756,7 @@
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,43 +783,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="28" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
@@ -848,18 +845,18 @@
         <v>4</v>
       </c>
       <c r="K2" s="30"/>
-      <c r="L2" s="25"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="30"/>
-      <c r="N2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="N2" s="28"/>
+      <c r="R2" s="28"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <f ca="1">M3</f>
         <v>1719783180000.0002</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>33</v>
+      <c r="B3" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="11">
         <v>2</v>
@@ -909,8 +906,8 @@
         <f t="shared" ref="A4:A67" ca="1" si="0">M4</f>
         <v>1719783150000</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>33</v>
+      <c r="B4" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="C4" s="11">
         <v>3</v>
@@ -968,8 +965,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719783120000</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>34</v>
+      <c r="B5" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -1024,8 +1021,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719783089999.9998</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>35</v>
+      <c r="B6" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="11">
         <v>10</v>
@@ -1064,7 +1061,7 @@
         <v>1719783089999.9998</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R6" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1076,8 +1073,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719782400000.0002</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>35</v>
+      <c r="B7" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="11">
         <v>5</v>
@@ -1108,7 +1105,7 @@
         <v>1719782400000.0002</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P7" s="18"/>
       <c r="R7" s="24" t="str">
@@ -1121,8 +1118,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719782220000.0002</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>34</v>
+      <c r="B8" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="11">
         <v>6</v>
@@ -1153,7 +1150,7 @@
         <v>1719782220000.0002</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P8" s="19">
         <v>45450.999988425923</v>
@@ -1168,8 +1165,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719782040000.0002</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>33</v>
+      <c r="B9" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="11">
         <v>4</v>
@@ -1200,7 +1197,7 @@
         <v>1719782040000.0002</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P9" s="17">
         <f>(P8-$Q$5-0.875)*86400*1000</f>
@@ -1216,8 +1213,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719781860000.0002</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>34</v>
+      <c r="B10" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="11">
         <v>7</v>
@@ -1247,12 +1244,12 @@
         <f t="shared" ca="1" si="2"/>
         <v>1719781860000.0002</v>
       </c>
-      <c r="N10" s="21" t="s">
-        <v>29</v>
+      <c r="N10" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="R10" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>{ id: 1719781860000, email: "aluno2@gmail.com", status: "cancelado" , carrinho: [ { nome: "Hamburgão", quantidade: 1, preco: 6.5 }, ] },</v>
+        <v>{ id: 1719781860000, email: "aluno2@gmail.com", status: "finalizado" , carrinho: [ { nome: "Hamburgão", quantidade: 1, preco: 6.5 }, ] },</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1260,8 +1257,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719781680000.0002</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>35</v>
+      <c r="B11" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="C11" s="11">
         <v>4</v>
@@ -1300,7 +1297,7 @@
         <v>1719781680000.0002</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R11" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1312,8 +1309,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719781500000.0002</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>34</v>
+      <c r="B12" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="11">
         <v>10</v>
@@ -1352,7 +1349,7 @@
         <v>1719781500000.0002</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R12" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1364,8 +1361,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719696780000.0002</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>33</v>
+      <c r="B13" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -1396,7 +1393,7 @@
         <v>1719696780000.0002</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R13" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1408,8 +1405,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719696750000</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>33</v>
+      <c r="B14" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="2">
         <v>8</v>
@@ -1448,7 +1445,7 @@
         <v>1719696750000</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R14" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1460,8 +1457,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719696720000</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>34</v>
+      <c r="B15" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>9</v>
@@ -1492,7 +1489,7 @@
         <v>1719696720000</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R15" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1504,8 +1501,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719696689999.9998</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>35</v>
+      <c r="B16" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="2">
         <v>11</v>
@@ -1544,7 +1541,7 @@
         <v>1719696689999.9998</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R16" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1556,8 +1553,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>1719696000000.0002</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>35</v>
+      <c r="B17" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="C17" s="2">
         <v>15</v>
@@ -1596,7 +1593,7 @@
         <v>1719696000000.0002</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R17" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1609,7 +1606,7 @@
         <v>1719610380000.0002</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="11">
         <v>16</v>
@@ -1640,7 +1637,7 @@
         <v>1719610380000.0002</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P18" s="3"/>
       <c r="R18" s="24" t="str">
@@ -1654,7 +1651,7 @@
         <v>1719610350000</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="11">
         <v>4</v>
@@ -1693,7 +1690,7 @@
         <v>1719610350000</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="3"/>
       <c r="R19" s="24" t="str">
@@ -1707,7 +1704,7 @@
         <v>1719610320000</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="11">
         <v>2</v>
@@ -1738,7 +1735,7 @@
         <v>1719610320000</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R20" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1751,7 +1748,7 @@
         <v>1719610289999.9998</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="11">
         <v>14</v>
@@ -1782,7 +1779,7 @@
         <v>1719610289999.9998</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R21" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1795,7 +1792,7 @@
         <v>1719609600000.0002</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="11">
         <v>5</v>
@@ -1826,7 +1823,7 @@
         <v>1719609600000.0002</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P22" s="23"/>
       <c r="R22" s="24" t="str">
@@ -1840,7 +1837,7 @@
         <v>1719523980000.0002</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2">
         <v>6</v>
@@ -1871,7 +1868,7 @@
         <v>1719523980000.0002</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R23" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1884,7 +1881,7 @@
         <v>1719523950000</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2">
         <v>7</v>
@@ -1923,7 +1920,7 @@
         <v>1719523950000</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R24" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1936,7 +1933,7 @@
         <v>1719523920000</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2">
         <v>5</v>
@@ -1966,12 +1963,12 @@
         <f t="shared" ca="1" si="2"/>
         <v>1719523920000</v>
       </c>
-      <c r="N25" s="21" t="s">
-        <v>29</v>
+      <c r="N25" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="R25" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>{ id: 1719523920000, email: "aluno2@gmail.com", status: "cancelado" , carrinho: [ { nome: "Pão de Queijo Recheado", quantidade: 1, preco: 5 }, ] },</v>
+        <v>{ id: 1719523920000, email: "aluno2@gmail.com", status: "finalizado" , carrinho: [ { nome: "Pão de Queijo Recheado", quantidade: 1, preco: 5 }, ] },</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -1980,7 +1977,7 @@
         <v>1719523889999.9998</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
@@ -2011,7 +2008,7 @@
         <v>1719523889999.9998</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R26" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2024,7 +2021,7 @@
         <v>1719523200000.0002</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -2063,7 +2060,7 @@
         <v>1719523200000.0002</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R27" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2076,7 +2073,7 @@
         <v>1719437580000.0002</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="11">
         <v>7</v>
@@ -2107,7 +2104,7 @@
         <v>1719437580000.0002</v>
       </c>
       <c r="N28" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R28" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2120,7 +2117,7 @@
         <v>1719437550000</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="11">
         <v>10</v>
@@ -2151,7 +2148,7 @@
         <v>1719437550000</v>
       </c>
       <c r="N29" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R29" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2164,7 +2161,7 @@
         <v>1719437520000</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="11">
         <v>4</v>
@@ -2203,7 +2200,7 @@
         <v>1719437520000</v>
       </c>
       <c r="N30" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R30" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2216,7 +2213,7 @@
         <v>1719437489999.9998</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="11">
         <v>15</v>
@@ -2247,7 +2244,7 @@
         <v>1719437489999.9998</v>
       </c>
       <c r="N31" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R31" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2260,7 +2257,7 @@
         <v>1719436800000.0002</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="11">
         <v>6</v>
@@ -2291,7 +2288,7 @@
         <v>1719436800000.0002</v>
       </c>
       <c r="N32" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R32" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2304,7 +2301,7 @@
         <v>1719178380000.0002</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2">
         <v>8</v>
@@ -2335,7 +2332,7 @@
         <v>1719178380000.0002</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R33" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2348,7 +2345,7 @@
         <v>1719178350000</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -2387,7 +2384,7 @@
         <v>1719178350000</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R34" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2400,7 +2397,7 @@
         <v>1719178320000</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2">
         <v>14</v>
@@ -2431,7 +2428,7 @@
         <v>1719178320000</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R35" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2444,7 +2441,7 @@
         <v>1719178289999.9998</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="2">
         <v>14</v>
@@ -2475,7 +2472,7 @@
         <v>1719178289999.9998</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R36" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2488,7 +2485,7 @@
         <v>1719177600000.0002</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="2">
         <v>5</v>
@@ -2519,7 +2516,7 @@
         <v>1719177600000.0002</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R37" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2532,7 +2529,7 @@
         <v>1719091980000.0002</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" s="11">
         <v>3</v>
@@ -2571,7 +2568,7 @@
         <v>1719091980000.0002</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R38" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2584,7 +2581,7 @@
         <v>1719091950000</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="11">
         <v>5</v>
@@ -2615,7 +2612,7 @@
         <v>1719091950000</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R39" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2628,7 +2625,7 @@
         <v>1719091920000</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="11">
         <v>14</v>
@@ -2659,7 +2656,7 @@
         <v>1719091920000</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R40" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2672,7 +2669,7 @@
         <v>1719091889999.9998</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="11">
         <v>7</v>
@@ -2703,7 +2700,7 @@
         <v>1719091889999.9998</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R41" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2716,7 +2713,7 @@
         <v>1719091200000.0002</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="11">
         <v>10</v>
@@ -2754,12 +2751,12 @@
         <f t="shared" ca="1" si="2"/>
         <v>1719091200000.0002</v>
       </c>
-      <c r="N42" s="21" t="s">
-        <v>29</v>
+      <c r="N42" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="R42" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>{ id: 1719091200000, email: "aluno3@gmail.com", status: "cancelado" , carrinho: [ { nome: "Hambúrguer", quantidade: 1, preco: 12 }, { id: 12, descricao: "Refrigerante", quantidade: 1, preco: 6 }, ] },</v>
+        <v>{ id: 1719091200000, email: "aluno3@gmail.com", status: "finalizado" , carrinho: [ { nome: "Hambúrguer", quantidade: 1, preco: 12 }, { id: 12, descricao: "Refrigerante", quantidade: 1, preco: 6 }, ] },</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -2768,7 +2765,7 @@
         <v>1719005580000.0002</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" s="2">
         <v>4</v>
@@ -2799,7 +2796,7 @@
         <v>1719005580000.0002</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R43" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2812,7 +2809,7 @@
         <v>1719005550000</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C44" s="2">
         <v>14</v>
@@ -2843,7 +2840,7 @@
         <v>1719005550000</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R44" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2856,7 +2853,7 @@
         <v>1719005520000</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2">
         <v>4</v>
@@ -2887,7 +2884,7 @@
         <v>1719005520000</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R45" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2900,7 +2897,7 @@
         <v>1719005489999.9998</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="2">
         <v>3</v>
@@ -2939,7 +2936,7 @@
         <v>1719005489999.9998</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R46" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2952,7 +2949,7 @@
         <v>1719004800000.0002</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2">
         <v>8</v>
@@ -2983,7 +2980,7 @@
         <v>1719004800000.0002</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R47" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2996,7 +2993,7 @@
         <v>1718919180000.0002</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="11">
         <v>4</v>
@@ -3027,7 +3024,7 @@
         <v>1718919180000.0002</v>
       </c>
       <c r="N48" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R48" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3040,7 +3037,7 @@
         <v>1718919150000</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" s="11">
         <v>14</v>
@@ -3071,7 +3068,7 @@
         <v>1718919150000</v>
       </c>
       <c r="N49" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R49" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3084,7 +3081,7 @@
         <v>1718919120000</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C50" s="11">
         <v>7</v>
@@ -3123,7 +3120,7 @@
         <v>1718919120000</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R50" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3136,7 +3133,7 @@
         <v>1718919089999.9998</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="11">
         <v>10</v>
@@ -3167,7 +3164,7 @@
         <v>1718919089999.9998</v>
       </c>
       <c r="N51" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R51" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3180,7 +3177,7 @@
         <v>1718918400000.0002</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C52" s="11">
         <v>5</v>
@@ -3219,7 +3216,7 @@
         <v>1718918400000.0002</v>
       </c>
       <c r="N52" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R52" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3232,7 +3229,7 @@
         <v>1718832780000.0002</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" s="2">
         <v>10</v>
@@ -3263,7 +3260,7 @@
         <v>1718832780000.0002</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R53" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3276,7 +3273,7 @@
         <v>1718832750000</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2">
         <v>14</v>
@@ -3307,7 +3304,7 @@
         <v>1718832750000</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R54" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3320,7 +3317,7 @@
         <v>1718832720000</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C55" s="2">
         <v>4</v>
@@ -3351,7 +3348,7 @@
         <v>1718832720000</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R55" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3364,7 +3361,7 @@
         <v>1718832689999.9998</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" s="2">
         <v>15</v>
@@ -3403,7 +3400,7 @@
         <v>1718832689999.9998</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R56" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3416,7 +3413,7 @@
         <v>1718832000000.0002</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C57" s="2">
         <v>6</v>
@@ -3447,7 +3444,7 @@
         <v>1718832000000.0002</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R57" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3460,7 +3457,7 @@
         <v>1718573580000.0002</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C58" s="11">
         <v>4</v>
@@ -3491,7 +3488,7 @@
         <v>1718573580000.0002</v>
       </c>
       <c r="N58" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R58" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3504,7 +3501,7 @@
         <v>1718573550000</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="11">
         <v>1</v>
@@ -3535,7 +3532,7 @@
         <v>1718573550000</v>
       </c>
       <c r="N59" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R59" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3548,7 +3545,7 @@
         <v>1718573520000</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" s="11">
         <v>7</v>
@@ -3587,7 +3584,7 @@
         <v>1718573520000</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R60" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3600,7 +3597,7 @@
         <v>1718573489999.9998</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C61" s="11">
         <v>2</v>
@@ -3631,7 +3628,7 @@
         <v>1718573489999.9998</v>
       </c>
       <c r="N61" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R61" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3644,7 +3641,7 @@
         <v>1718572800000.0002</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C62" s="11">
         <v>15</v>
@@ -3675,7 +3672,7 @@
         <v>1718572800000.0002</v>
       </c>
       <c r="N62" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R62" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3688,7 +3685,7 @@
         <v>1718487180000.0002</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C63" s="2">
         <v>4</v>
@@ -3719,7 +3716,7 @@
         <v>1718487180000.0002</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R63" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3732,7 +3729,7 @@
         <v>1718487150000</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C64" s="2">
         <v>6</v>
@@ -3771,7 +3768,7 @@
         <v>1718487150000</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R64" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3784,7 +3781,7 @@
         <v>1718487120000</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C65" s="2">
         <v>5</v>
@@ -3815,7 +3812,7 @@
         <v>1718487120000</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R65" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3828,7 +3825,7 @@
         <v>1718487089999.9998</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C66" s="2">
         <v>3</v>
@@ -3867,7 +3864,7 @@
         <v>1718487089999.9998</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R66" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3880,7 +3877,7 @@
         <v>1718486400000.0002</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C67" s="2">
         <v>8</v>
@@ -3911,7 +3908,7 @@
         <v>1718486400000.0002</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R67" s="24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3924,7 +3921,7 @@
         <v>1718400780000.0002</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C68" s="11">
         <v>4</v>
@@ -3955,7 +3952,7 @@
         <v>1718400780000.0002</v>
       </c>
       <c r="N68" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R68" s="24" t="str">
         <f t="shared" ref="R68:R131" ca="1" si="22">CONCATENATE("{ id: ",A68,", email: """,B68,""", status: ","""",N68,""""," , carrinho: [ ", "{ nome: ","""",D68,"""",", quantidade: ",E68,", preco: ",SUBSTITUTE(F68,",",".")," },",IF(G68&lt;&gt;"",CONCATENATE(" { id: ",G68,", descricao: ","""",H68,"""",", quantidade: ",I68,", preco: ",SUBSTITUTE(J68,",",".")," },"),""), " ] },")</f>
@@ -3968,7 +3965,7 @@
         <v>1718400750000</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C69" s="11">
         <v>1</v>
@@ -3999,7 +3996,7 @@
         <v>1718400750000</v>
       </c>
       <c r="N69" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R69" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4012,7 +4009,7 @@
         <v>1718400720000</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C70" s="11">
         <v>5</v>
@@ -4051,7 +4048,7 @@
         <v>1718400720000</v>
       </c>
       <c r="N70" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R70" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4064,7 +4061,7 @@
         <v>1718400689999.9998</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C71" s="11">
         <v>2</v>
@@ -4095,7 +4092,7 @@
         <v>1718400689999.9998</v>
       </c>
       <c r="N71" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R71" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4108,7 +4105,7 @@
         <v>1718400000000.0002</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C72" s="11">
         <v>14</v>
@@ -4139,7 +4136,7 @@
         <v>1718400000000.0002</v>
       </c>
       <c r="N72" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R72" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4152,7 +4149,7 @@
         <v>1718314380000.0002</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C73" s="2">
         <v>4</v>
@@ -4183,7 +4180,7 @@
         <v>1718314380000.0002</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R73" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4196,7 +4193,7 @@
         <v>1718314350000</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C74" s="2">
         <v>8</v>
@@ -4235,7 +4232,7 @@
         <v>1718314350000</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R74" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4248,7 +4245,7 @@
         <v>1718314320000</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C75" s="2">
         <v>5</v>
@@ -4279,7 +4276,7 @@
         <v>1718314320000</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R75" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4292,7 +4289,7 @@
         <v>1718314289999.9998</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C76" s="2">
         <v>7</v>
@@ -4331,7 +4328,7 @@
         <v>1718314289999.9998</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R76" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4344,7 +4341,7 @@
         <v>1718313600000.0002</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C77" s="2">
         <v>8</v>
@@ -4375,7 +4372,7 @@
         <v>1718313600000.0002</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R77" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4388,7 +4385,7 @@
         <v>1718227980000.0002</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C78" s="11">
         <v>5</v>
@@ -4419,7 +4416,7 @@
         <v>1718227980000.0002</v>
       </c>
       <c r="N78" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R78" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4432,7 +4429,7 @@
         <v>1718227950000</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C79" s="11">
         <v>8</v>
@@ -4471,7 +4468,7 @@
         <v>1718227950000</v>
       </c>
       <c r="N79" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R79" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4484,7 +4481,7 @@
         <v>1718227920000</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C80" s="11">
         <v>9</v>
@@ -4515,7 +4512,7 @@
         <v>1718227920000</v>
       </c>
       <c r="N80" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R80" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4528,7 +4525,7 @@
         <v>1718227889999.9998</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C81" s="11">
         <v>11</v>
@@ -4567,7 +4564,7 @@
         <v>1718227889999.9998</v>
       </c>
       <c r="N81" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R81" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4580,7 +4577,7 @@
         <v>1718227200000.0002</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C82" s="11">
         <v>15</v>
@@ -4619,7 +4616,7 @@
         <v>1718227200000.0002</v>
       </c>
       <c r="N82" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R82" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4632,7 +4629,7 @@
         <v>1717968780000.0002</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C83" s="11">
         <v>4</v>
@@ -4663,7 +4660,7 @@
         <v>1717968780000.0002</v>
       </c>
       <c r="N83" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R83" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4676,7 +4673,7 @@
         <v>1717968750000</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C84" s="11">
         <v>1</v>
@@ -4707,7 +4704,7 @@
         <v>1717968750000</v>
       </c>
       <c r="N84" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R84" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4720,7 +4717,7 @@
         <v>1717968720000</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C85" s="11">
         <v>7</v>
@@ -4759,7 +4756,7 @@
         <v>1717968720000</v>
       </c>
       <c r="N85" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R85" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4772,7 +4769,7 @@
         <v>1717968689999.9998</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C86" s="11">
         <v>2</v>
@@ -4803,7 +4800,7 @@
         <v>1717968689999.9998</v>
       </c>
       <c r="N86" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R86" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4816,7 +4813,7 @@
         <v>1717968000000.0002</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C87" s="11">
         <v>15</v>
@@ -4847,7 +4844,7 @@
         <v>1717968000000.0002</v>
       </c>
       <c r="N87" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R87" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4860,7 +4857,7 @@
         <v>1717882380000.0002</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C88" s="2">
         <v>4</v>
@@ -4891,7 +4888,7 @@
         <v>1717882380000.0002</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R88" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4904,7 +4901,7 @@
         <v>1717882350000</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C89" s="2">
         <v>6</v>
@@ -4943,7 +4940,7 @@
         <v>1717882350000</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R89" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4956,7 +4953,7 @@
         <v>1717882320000</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C90" s="2">
         <v>5</v>
@@ -4987,7 +4984,7 @@
         <v>1717882320000</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R90" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5000,7 +4997,7 @@
         <v>1717882289999.9998</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C91" s="2">
         <v>3</v>
@@ -5039,7 +5036,7 @@
         <v>1717882289999.9998</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R91" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5052,7 +5049,7 @@
         <v>1717881600000.0002</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C92" s="2">
         <v>8</v>
@@ -5083,7 +5080,7 @@
         <v>1717881600000.0002</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R92" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5096,7 +5093,7 @@
         <v>1717795980000.0002</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C93" s="11">
         <v>4</v>
@@ -5127,7 +5124,7 @@
         <v>1717795980000.0002</v>
       </c>
       <c r="N93" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R93" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5140,7 +5137,7 @@
         <v>1717795950000</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C94" s="11">
         <v>1</v>
@@ -5171,7 +5168,7 @@
         <v>1717795950000</v>
       </c>
       <c r="N94" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R94" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5184,7 +5181,7 @@
         <v>1717795920000</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C95" s="11">
         <v>5</v>
@@ -5223,7 +5220,7 @@
         <v>1717795920000</v>
       </c>
       <c r="N95" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R95" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5236,7 +5233,7 @@
         <v>1717795889999.9998</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C96" s="11">
         <v>2</v>
@@ -5267,7 +5264,7 @@
         <v>1717795889999.9998</v>
       </c>
       <c r="N96" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R96" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5280,7 +5277,7 @@
         <v>1717795200000.0002</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C97" s="11">
         <v>14</v>
@@ -5311,7 +5308,7 @@
         <v>1717795200000.0002</v>
       </c>
       <c r="N97" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R97" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5324,7 +5321,7 @@
         <v>1717709580000.0002</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C98" s="2">
         <v>4</v>
@@ -5355,7 +5352,7 @@
         <v>1717709580000.0002</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R98" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5368,7 +5365,7 @@
         <v>1717709550000</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C99" s="2">
         <v>8</v>
@@ -5407,7 +5404,7 @@
         <v>1717709550000</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R99" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5420,7 +5417,7 @@
         <v>1717709520000</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C100" s="2">
         <v>5</v>
@@ -5451,7 +5448,7 @@
         <v>1717709520000</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R100" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5464,7 +5461,7 @@
         <v>1717709489999.9998</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C101" s="2">
         <v>7</v>
@@ -5503,7 +5500,7 @@
         <v>1717709489999.9998</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R101" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5516,7 +5513,7 @@
         <v>1717708800000.0002</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C102" s="2">
         <v>8</v>
@@ -5547,7 +5544,7 @@
         <v>1717708800000.0002</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R102" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5560,7 +5557,7 @@
         <v>1717623180000.0002</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C103" s="11">
         <v>5</v>
@@ -5591,7 +5588,7 @@
         <v>1717623180000.0002</v>
       </c>
       <c r="N103" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R103" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5604,7 +5601,7 @@
         <v>1717623150000</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C104" s="11">
         <v>8</v>
@@ -5643,7 +5640,7 @@
         <v>1717623150000</v>
       </c>
       <c r="N104" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R104" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5656,7 +5653,7 @@
         <v>1717623120000</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C105" s="11">
         <v>9</v>
@@ -5687,7 +5684,7 @@
         <v>1717623120000</v>
       </c>
       <c r="N105" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R105" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5700,7 +5697,7 @@
         <v>1717623089999.9998</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C106" s="11">
         <v>11</v>
@@ -5739,7 +5736,7 @@
         <v>1717623089999.9998</v>
       </c>
       <c r="N106" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R106" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5752,7 +5749,7 @@
         <v>1717622400000.0002</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C107" s="11">
         <v>15</v>
@@ -5791,7 +5788,7 @@
         <v>1717622400000.0002</v>
       </c>
       <c r="N107" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R107" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5804,7 +5801,7 @@
         <v>1717363980000.0002</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C108" s="11">
         <v>4</v>
@@ -5835,7 +5832,7 @@
         <v>1717363980000.0002</v>
       </c>
       <c r="N108" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R108" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5848,7 +5845,7 @@
         <v>1717363950000</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C109" s="11">
         <v>1</v>
@@ -5879,7 +5876,7 @@
         <v>1717363950000</v>
       </c>
       <c r="N109" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R109" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5892,7 +5889,7 @@
         <v>1717363920000</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C110" s="11">
         <v>7</v>
@@ -5931,7 +5928,7 @@
         <v>1717363920000</v>
       </c>
       <c r="N110" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R110" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5944,7 +5941,7 @@
         <v>1717363889999.9998</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C111" s="11">
         <v>2</v>
@@ -5975,7 +5972,7 @@
         <v>1717363889999.9998</v>
       </c>
       <c r="N111" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R111" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -5988,7 +5985,7 @@
         <v>1717363200000.0002</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C112" s="11">
         <v>15</v>
@@ -6019,7 +6016,7 @@
         <v>1717363200000.0002</v>
       </c>
       <c r="N112" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R112" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6032,7 +6029,7 @@
         <v>1717277580000.0002</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C113" s="2">
         <v>4</v>
@@ -6063,7 +6060,7 @@
         <v>1717277580000.0002</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R113" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6076,7 +6073,7 @@
         <v>1717277550000</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C114" s="2">
         <v>6</v>
@@ -6115,7 +6112,7 @@
         <v>1717277550000</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R114" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6128,7 +6125,7 @@
         <v>1717277520000</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C115" s="2">
         <v>5</v>
@@ -6159,7 +6156,7 @@
         <v>1717277520000</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R115" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6172,7 +6169,7 @@
         <v>1717277489999.9998</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C116" s="2">
         <v>3</v>
@@ -6211,7 +6208,7 @@
         <v>1717277489999.9998</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R116" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6224,7 +6221,7 @@
         <v>1717276800000.0002</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C117" s="2">
         <v>8</v>
@@ -6255,7 +6252,7 @@
         <v>1717276800000.0002</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R117" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6268,7 +6265,7 @@
         <v>1717191180000.0002</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C118" s="11">
         <v>4</v>
@@ -6299,7 +6296,7 @@
         <v>1717191180000.0002</v>
       </c>
       <c r="N118" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R118" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6312,7 +6309,7 @@
         <v>1717191150000</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C119" s="11">
         <v>1</v>
@@ -6343,7 +6340,7 @@
         <v>1717191150000</v>
       </c>
       <c r="N119" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R119" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6356,7 +6353,7 @@
         <v>1717191120000</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C120" s="11">
         <v>5</v>
@@ -6395,7 +6392,7 @@
         <v>1717191120000</v>
       </c>
       <c r="N120" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R120" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6408,7 +6405,7 @@
         <v>1717191089999.9998</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C121" s="11">
         <v>2</v>
@@ -6439,7 +6436,7 @@
         <v>1717191089999.9998</v>
       </c>
       <c r="N121" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R121" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6452,7 +6449,7 @@
         <v>1717190400000.0002</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C122" s="11">
         <v>14</v>
@@ -6483,7 +6480,7 @@
         <v>1717190400000.0002</v>
       </c>
       <c r="N122" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R122" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6496,7 +6493,7 @@
         <v>1717104780000.0002</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C123" s="2">
         <v>4</v>
@@ -6527,7 +6524,7 @@
         <v>1717104780000.0002</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R123" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6540,7 +6537,7 @@
         <v>1717104750000</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C124" s="2">
         <v>8</v>
@@ -6579,7 +6576,7 @@
         <v>1717104750000</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R124" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6592,7 +6589,7 @@
         <v>1717104720000</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C125" s="2">
         <v>5</v>
@@ -6623,7 +6620,7 @@
         <v>1717104720000</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R125" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6636,7 +6633,7 @@
         <v>1717104689999.9998</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C126" s="2">
         <v>7</v>
@@ -6675,7 +6672,7 @@
         <v>1717104689999.9998</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R126" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6688,7 +6685,7 @@
         <v>1717104000000.0002</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C127" s="2">
         <v>8</v>
@@ -6719,7 +6716,7 @@
         <v>1717104000000.0002</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R127" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6732,7 +6729,7 @@
         <v>1717018380000.0002</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C128" s="11">
         <v>5</v>
@@ -6763,7 +6760,7 @@
         <v>1717018380000.0002</v>
       </c>
       <c r="N128" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R128" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6776,7 +6773,7 @@
         <v>1717018350000</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C129" s="11">
         <v>8</v>
@@ -6815,7 +6812,7 @@
         <v>1717018350000</v>
       </c>
       <c r="N129" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R129" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6828,7 +6825,7 @@
         <v>1717018320000</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C130" s="11">
         <v>9</v>
@@ -6859,7 +6856,7 @@
         <v>1717018320000</v>
       </c>
       <c r="N130" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R130" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6872,7 +6869,7 @@
         <v>1717018289999.9998</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C131" s="11">
         <v>11</v>
@@ -6911,7 +6908,7 @@
         <v>1717018289999.9998</v>
       </c>
       <c r="N131" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R131" s="24" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -6924,7 +6921,7 @@
         <v>1717017600000.0002</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C132" s="11">
         <v>15</v>
@@ -6963,9 +6960,9 @@
         <v>1717017600000.0002</v>
       </c>
       <c r="N132" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="R132" s="33" t="str">
+        <v>30</v>
+      </c>
+      <c r="R132" s="27" t="str">
         <f t="shared" ref="R132" ca="1" si="39">CONCATENATE("{ id: ",A132,", email: """,B132,""", status: ","""",N132,""""," , carrinho: [ ", "{ nome: ","""",D132,"""",", quantidade: ",E132,", preco: ",SUBSTITUTE(F132,",",".")," },",IF(G132&lt;&gt;"",CONCATENATE(" { id: ",G132,", descricao: ","""",H132,"""",", quantidade: ",I132,", preco: ",SUBSTITUTE(J132,",",".")," },"),""), " ] },")</f>
         <v>{ id: 1717017600000, email: "aluno3@gmail.com", status: "finalizado" , carrinho: [ { nome: "Água", quantidade: 1, preco: 4.5 }, { id: 17, descricao: "Bombom", quantidade: 1, preco: 3 }, ] },</v>
       </c>

</xml_diff>